<commit_message>
- Ajouter un classeur avec les produits par clients pour le producteur sur la factures producteurs ( indispensable pour les producteurs qui prépare leurs panier)
</commit_message>
<xml_diff>
--- a/src/Stolons/wwwroot/bills/Stolons/2016_25.xlsx
+++ b/src/Stolons/wwwroot/bills/Stolons/2016_25.xlsx
@@ -6,13 +6,14 @@
   </bookViews>
   <sheets>
     <sheet name="1 (PARAVEL)" sheetId="1" r:id="rId1"/>
+    <sheet name="2 (MICHON)" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Facture</t>
   </si>
@@ -93,6 +94,24 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL : </t>
+  </si>
+  <si>
+    <t>MICHON</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>4 pièces</t>
+  </si>
+  <si>
+    <t>4 Kg</t>
+  </si>
+  <si>
+    <t>2 pièces</t>
+  </si>
+  <si>
+    <t>1 Kg</t>
   </si>
 </sst>
 </file>
@@ -516,4 +535,318 @@
   </mergeCells>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" view="pageLayout"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="19.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="11.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="11.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="11">
+        <f ref="F6:F7" t="shared" si="1">F16</f>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="10">
+        <f>4*D12</f>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.9900000095367432</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="10">
+        <f>4*D13</f>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10">
+        <f>2*D14</f>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="10">
+        <f>2*D15</f>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="10">
+        <f>SUBTOTAL(9,F12:F15)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:C8"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:F11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>